<commit_message>
updated file structure for training material
</commit_message>
<xml_diff>
--- a/r-project-mgmt-repro/docs/Book1.xlsx
+++ b/r-project-mgmt-repro/docs/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joubertd/Documents/nihl-intro-r-series/r-project-mgmt-repro/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03804E28-BEC4-9846-A627-3999D01E5BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30351A5D-F139-5449-BE1B-E1E5A4FB825B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1360" windowWidth="17820" windowHeight="14260" xr2:uid="{4E2C795C-286A-7E4F-8C3A-E58F96518E62}"/>
+    <workbookView xWindow="1780" yWindow="3400" windowWidth="21940" windowHeight="11980" xr2:uid="{4E2C795C-286A-7E4F-8C3A-E58F96518E62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -416,7 +416,7 @@
     <col min="5" max="5" width="46.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:5" ht="162" x14ac:dyDescent="0.3">
+    <row r="1" spans="5:5" ht="112" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>